<commit_message>
to deliver, actualizado casos de prueba y documentación
</commit_message>
<xml_diff>
--- a/documentacion_usuario/Casos de prueba.xlsx
+++ b/documentacion_usuario/Casos de prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario.diaz.rodriguez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario.diaz.rodriguez\PycharmProjects\CitiBank_Boletos\documentacion_usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F31F75E-0E93-45D7-A536-B9F382B7EDCD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1AAD5E-A178-4E05-AF19-AEB8764D800A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,13 +184,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>922778</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>180951</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -228,13 +228,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>6876193</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>85529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -272,13 +272,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2550983</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>169622</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -316,13 +316,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1561924</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>76181</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -360,13 +360,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1257154</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>76177</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -404,13 +404,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1838325</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4952611</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -447,15 +447,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2562225</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:colOff>1847850</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4229100</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:colOff>5010150</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -478,8 +478,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4981575" y="7753351"/>
-          <a:ext cx="1666875" cy="1276350"/>
+          <a:off x="4267200" y="7648576"/>
+          <a:ext cx="3162300" cy="1276350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,13 +492,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>5553076</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -536,13 +536,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>623887</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>862012</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>19053</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -596,13 +596,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1409699</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1666874</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -656,13 +656,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3048000</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3419476</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -715,15 +715,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4410075</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:colOff>5124450</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>5153025</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:colOff>5410200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -738,8 +738,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6829425" y="8058149"/>
-          <a:ext cx="742950" cy="447675"/>
+          <a:off x="7543800" y="8029574"/>
+          <a:ext cx="285750" cy="447675"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -776,13 +776,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1802100</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>45287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2338323</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>36068</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -839,13 +839,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1904506</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>28387</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -883,13 +883,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3611850</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>54815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4148073</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>45596</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -946,13 +946,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1857374</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1069,7 +1069,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2190750</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -1124,13 +1124,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2809874</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>6762749</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1199,13 +1199,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1781175</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2000251</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1259,13 +1259,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1800225</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2019301</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1319,13 +1319,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1819275</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2038351</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1379,13 +1379,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3476625</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>6243130</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1417,6 +1417,291 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4752975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B6D5F6-1EF4-42D3-AA48-24278E3246FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2428875" y="4772025"/>
+          <a:ext cx="4743450" cy="2419349"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Validación de campos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>número de boleto: numérico</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>enteprise_id : alfanumérico</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>cpf o cnpj, numérico, la aplicación en virtud de la longitud de este campo es capaz de determinar el tipo de que se trata.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>product: numérico, valores permitidos (100 o 180)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>account_number: numérico</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>address: alfanumérico</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>state: cadena</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>city : cadena</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>zip_code: 8 dígitos</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>emision_date/ due_date: fecha formato dd/mm/yyyy</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>amount : numérico</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1719,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:B85"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,213 +2019,210 @@
     <col min="5" max="5" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+      <c r="B87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A77:B78"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>